<commit_message>
Bugs resolus et fonctionnalités ajoutées
</commit_message>
<xml_diff>
--- a/code/BRP_front_end/src/main/webapp/export_files/Exports/Gustavo 2_23/Gustavo 2_DPGF.xlsx
+++ b/code/BRP_front_end/src/main/webapp/export_files/Exports/Gustavo 2_23/Gustavo 2_DPGF.xlsx
@@ -14,6 +14,7 @@
   </bookViews>
   <sheets>
     <sheet name="Garde" sheetId="6" r:id="rId1"/>
+    <sheet name="Lot_1_" r:id="rId5" sheetId="7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Garde!$A$1:$D$41</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>MARCHES PUBLICS DE TRAVAUX</t>
   </si>
@@ -80,13 +81,76 @@
   <si>
     <t>Vérificateur :</t>
   </si>
+  <si>
+    <t>N° art. CCTP</t>
+  </si>
+  <si>
+    <t>DESIGNATION</t>
+  </si>
+  <si>
+    <t>DESCRIPTION SOMMAIRE 
+(se référer à l'article du CCTP)</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>Montant HT</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUS-TOTAL </t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>II.1</t>
+  </si>
+  <si>
+    <t>II.2</t>
+  </si>
+  <si>
+    <t>Bac acier plein support d’étanchéité</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>II.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECAPITULATIF </t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>PRIX TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTANT TOTAL H.T </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="13">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00€"/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,16 +239,118 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="8DB4E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="8DB4E2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="BFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="BFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -320,11 +486,170 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <right style="thin"/>
+    </border>
+    <border>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="medium"/>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,6 +825,67 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="20" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="20" xfId="0" applyFill="true" applyFont="true" applyBorder="true" applyNumberFormat="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="20" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyBorder="true" applyFont="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="20" xfId="0" applyBorder="true" applyFont="true" applyFill="true" applyNumberFormat="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="20" xfId="0" applyFill="true" applyFont="true" applyBorder="true" applyNumberFormat="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="31" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="true" applyNumberFormat="true" applyBorder="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="31" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyNumberFormat="true" applyBorder="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="9" borderId="20" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1285,4 +1671,362 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="12.0625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.921875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="28.09375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="3.53515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.9296875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="7.16015625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.75" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="60">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s" s="60">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s" s="60">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s" s="60">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s" s="60">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s" s="60">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s" s="60">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s" s="61">
+        <v>23</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s" s="63">
+        <v>23</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F10" s="70" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G10" s="70" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="73" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F11" s="74" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="G11" s="74" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75" t="n">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15">
+      <c r="A15" t="s" s="76">
+        <v>31</v>
+      </c>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="77">
+        <v>23</v>
+      </c>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="78">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s" s="78">
+        <v>16</v>
+      </c>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" t="s" s="78">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" t="s" s="80">
+        <v>23</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="81">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s" s="81">
+        <v>16</v>
+      </c>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" t="s" s="81">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="82">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s" s="82">
+        <v>23</v>
+      </c>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" t="n" s="82">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="83">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s" s="83">
+        <v>28</v>
+      </c>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" t="n" s="83">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="84">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s" s="84">
+        <v>28</v>
+      </c>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" t="n" s="84">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85" t="n">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86" t="n">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="28"/>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A27:F27"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>